<commit_message>
feat(modify docs): Update the docs folder
</commit_message>
<xml_diff>
--- a/docs/diccionario_datos.xlsx
+++ b/docs/diccionario_datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Documents\GitHub - Projects\Doc-UP-AlejandroJaimes\BDI-GB-ZOO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E69C1A-C0CC-4560-88CF-4AEE407A995C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9250BF-D185-4D3B-B89D-F577A70BA89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DICCIONARIO DE DATOS" sheetId="12" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="HABITAT" sheetId="7" r:id="rId8"/>
     <sheet name="UBICACION" sheetId="8" r:id="rId9"/>
     <sheet name="CLIMA" sheetId="9" r:id="rId10"/>
-    <sheet name="VISITANTES" sheetId="10" r:id="rId11"/>
-    <sheet name="HABITAT_VISITANTES" sheetId="11" r:id="rId12"/>
+    <sheet name="TIPO_VISITANTES" sheetId="13" r:id="rId11"/>
+    <sheet name="VISITANTES" sheetId="10" r:id="rId12"/>
+    <sheet name="HABITAT_VISITANTES" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="139">
   <si>
     <t>Campo</t>
   </si>
@@ -461,6 +462,48 @@
   </si>
   <si>
     <t>(10,2)</t>
+  </si>
+  <si>
+    <t>CostoBase</t>
+  </si>
+  <si>
+    <t>Costo base de entrada para acceder a cada hábitat del zoológico, expresado en moneda local. Este valor representa el precio estándar antes de aplicar descuentos según el tipo de visitante</t>
+  </si>
+  <si>
+    <t>Identificador único del tipo de visitante.</t>
+  </si>
+  <si>
+    <t>Nombre descriptivo del tipo de visitante (e.g., Adulto, Menor de edad, Estudiante).</t>
+  </si>
+  <si>
+    <t>Porcentaje de descuento aplicable a este tipo de visitante. Representado como un valor entre 0 y 100.</t>
+  </si>
+  <si>
+    <t>Descuento</t>
+  </si>
+  <si>
+    <t>(5,2)</t>
+  </si>
+  <si>
+    <t>TIPO_VISITANTES</t>
+  </si>
+  <si>
+    <t>Almacena los distintos tipos de visitantes que acceden al zoológico, como Adulto, Menor de edad y Estudiante, junto con el porcentaje de descuento aplicable a cada tipo. Esta información permite calcular tarifas ajustadas según el tipo de visitante.</t>
+  </si>
+  <si>
+    <t>IDTipoVisitantes</t>
+  </si>
+  <si>
+    <t>Identificador del tipo de visitantes.</t>
+  </si>
+  <si>
+    <t>CostoFinal</t>
+  </si>
+  <si>
+    <t>NOT NULL (DEFAULT)</t>
+  </si>
+  <si>
+    <t>Costo final calculada del descuento por el tipo de visitante, calculado con la funcion calcular_descuento() que aplica la formula Costo Final=Costo Base×(1−Descuento/100)</t>
   </si>
 </sst>
 </file>
@@ -578,7 +621,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,12 +670,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -662,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -717,8 +754,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1162,19 +1215,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339450DB-CBA5-4825-8615-F0DCB265D8CD}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:H16"/>
+    <sheetView topLeftCell="A22" zoomScale="116" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="32.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19" t="s">
         <v>76</v>
       </c>
@@ -1186,7 +1239,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
         <v>66</v>
       </c>
@@ -1198,7 +1251,7 @@
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
     </row>
-    <row r="3" spans="1:8" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1265,7 @@
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
     </row>
-    <row r="4" spans="1:8" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -1226,7 +1279,7 @@
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1240,7 +1293,7 @@
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:8" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -1254,7 +1307,7 @@
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -1268,7 +1321,7 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1282,7 +1335,7 @@
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A9" s="22" t="s">
         <v>67</v>
       </c>
@@ -1294,7 +1347,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -1308,7 +1361,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1322,7 +1375,7 @@
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
@@ -1336,7 +1389,7 @@
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
@@ -1350,7 +1403,7 @@
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A14" s="22" t="s">
         <v>82</v>
       </c>
@@ -1362,7 +1415,7 @@
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>83</v>
       </c>
@@ -1378,7 +1431,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" ht="201.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
@@ -1395,7 +1448,7 @@
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>86</v>
       </c>
@@ -1406,13 +1459,13 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="25" t="str">
-        <f t="shared" ref="F17:F26" si="0">CONCATENATE(A17,"_LINK")</f>
+        <f t="shared" ref="F17:F27" si="0">CONCATENATE(A17,"_LINK")</f>
         <v>CUIDADOR_LINK</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>87</v>
       </c>
@@ -1429,7 +1482,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>88</v>
       </c>
@@ -1446,7 +1499,7 @@
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>89</v>
       </c>
@@ -1463,7 +1516,7 @@
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
     </row>
-    <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>90</v>
       </c>
@@ -1480,7 +1533,7 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:8" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>91</v>
       </c>
@@ -1497,7 +1550,7 @@
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>92</v>
       </c>
@@ -1514,7 +1567,7 @@
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
     </row>
-    <row r="24" spans="1:8" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
@@ -1531,76 +1584,95 @@
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="1:8" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>VISITANTES_LINK</v>
+        <f t="shared" ref="F25" si="1">CONCATENATE(A25,"_LINK")</f>
+        <v>TIPO_VISITANTES_LINK</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="1:8" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
       <c r="F26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>HABITAT_VISITANTES_LINK</v>
+        <v>VISITANTES_LINK</v>
       </c>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
     </row>
-    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+    <row r="27" spans="1:8" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>HABITAT_VISITANTES_LINK</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="23"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="B29" s="23"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="41">
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="F25:H25"/>
-    <mergeCell ref="B26:E26"/>
     <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F27:H27"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="B23:E23"/>
@@ -1608,7 +1680,7 @@
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="B13:H13"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:H15"/>
@@ -1622,7 +1694,7 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:H3"/>
@@ -1646,8 +1718,9 @@
     <hyperlink ref="F22:H22" location="HABITAT!A1" display="HABITAT!A1" xr:uid="{EA91EF00-DA2F-4E00-A5D4-0C1085EBEEBD}"/>
     <hyperlink ref="F23:H23" location="UBICACION!A1" display="UBICACION!A1" xr:uid="{D55219A8-4FD7-4064-9327-347592192A6E}"/>
     <hyperlink ref="F24:H24" location="CLIMA!A1" display="CLIMA!A1" xr:uid="{F64C0BF4-3B73-43FB-9793-F7181E1241EE}"/>
-    <hyperlink ref="F25:H25" location="VISITANTES!A1" display="VISITANTES!A1" xr:uid="{6A052436-EAC5-44FE-9A66-0894D7AFE2D5}"/>
-    <hyperlink ref="F26:H26" location="HABITAT_VISITANTES!A1" display="HABITAT_VISITANTES!A1" xr:uid="{5D5A4D0B-FAC0-4239-9056-4A34635EA186}"/>
+    <hyperlink ref="F26:H26" location="VISITANTES!A1" display="VISITANTES!A1" xr:uid="{6A052436-EAC5-44FE-9A66-0894D7AFE2D5}"/>
+    <hyperlink ref="F27:H27" location="HABITAT_VISITANTES!A1" display="HABITAT_VISITANTES!A1" xr:uid="{5D5A4D0B-FAC0-4239-9056-4A34635EA186}"/>
+    <hyperlink ref="F25:H25" location="TIPO_VISITANTES!A1" display="TIPO_VISITANTES!A1" xr:uid="{C6CAA7F9-AD1A-4879-B9E9-5DCA400104BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1666,16 +1739,16 @@
       <selection activeCell="E3" sqref="B1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1709,7 +1782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1732,6 +1805,99 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E833B78-DC58-45CB-81FE-BE4A0FF3FA6D}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -1739,19 +1905,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1785,7 +1951,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1802,21 +1968,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="12" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>50</v>
+      <c r="D4" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1824,23 +1990,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="127" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="26.7109375" customWidth="1"/>
+    <col min="1" max="5" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +2023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1874,7 +2040,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1891,7 +2057,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>51</v>
       </c>
@@ -1906,6 +2072,40 @@
       </c>
       <c r="E4" s="9" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1918,36 +2118,36 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1964,7 +2164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1981,7 +2181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>120</v>
       </c>
@@ -1998,7 +2198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>121</v>
       </c>
@@ -2015,7 +2215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -2032,7 +2232,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -2062,36 +2262,36 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="222" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2108,7 +2308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2125,7 +2325,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -2142,7 +2342,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
@@ -2159,7 +2359,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
@@ -2189,36 +2389,36 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="171" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2235,7 +2435,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2265,36 +2465,36 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2311,7 +2511,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2328,7 +2528,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>27</v>
       </c>
@@ -2345,7 +2545,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
@@ -2375,36 +2575,36 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="168" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2421,7 +2621,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>117</v>
       </c>
@@ -2438,7 +2638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>118</v>
       </c>
@@ -2469,36 +2669,36 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="176" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2515,7 +2715,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>113</v>
       </c>
@@ -2532,7 +2732,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -2549,7 +2749,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>84</v>
       </c>
@@ -2566,7 +2766,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" s="16"/>
     </row>
   </sheetData>
@@ -2580,39 +2780,39 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="162" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2629,7 +2829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2646,26 +2846,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>8</v>
@@ -2677,6 +2877,23 @@
         <v>112</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2692,37 +2909,37 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="233" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="233" workbookViewId="0">
+      <selection activeCell="E3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2739,7 +2956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>

</xml_diff>